<commit_message>
Start adding write var
</commit_message>
<xml_diff>
--- a/XLS_Kuka/Kuka_COMUNICATION.xlsx
+++ b/XLS_Kuka/Kuka_COMUNICATION.xlsx
@@ -814,8 +814,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>